<commit_message>
Internet Connectivity xlsx updated
</commit_message>
<xml_diff>
--- a/InternetConectivity.xlsx
+++ b/InternetConectivity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>CurrentLocation onClick</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>GoodBye and GoodLuck Rohit</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>01/10/11 case</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D27"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,6 +460,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
@@ -468,6 +477,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -485,6 +497,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -499,6 +514,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -512,10 +530,12 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
@@ -526,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
InternetConnectivity.xlsx udpated with nextStep
</commit_message>
<xml_diff>
--- a/InternetConectivity.xlsx
+++ b/InternetConectivity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>CurrentLocation onClick</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>01/10/11 case</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>shoes notification; but when internet available does not start location service clas</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +504,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -515,7 +521,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -548,6 +554,9 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
@@ -562,8 +571,14 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
@@ -578,6 +593,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
@@ -659,5 +677,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
InternetConnectivity possibly last updated :small_blue_diamond:
</commit_message>
<xml_diff>
--- a/InternetConectivity.xlsx
+++ b/InternetConectivity.xlsx
@@ -65,9 +65,6 @@
     <t>:)</t>
   </si>
   <si>
-    <t>Internet connectivity broadcase is on hold for the moment</t>
-  </si>
-  <si>
     <t>0--&gt;1</t>
   </si>
   <si>
@@ -116,7 +113,10 @@
     <t>ok</t>
   </si>
   <si>
-    <t>shoes notification; but when internet available does not start location service clas</t>
+    <t>Internet connectivity broadcast is on hold for the moment</t>
+  </si>
+  <si>
+    <t>shows notification; but when internet available does not start location service class</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -449,6 +449,7 @@
     <col min="2" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="55.26953125" customWidth="1"/>
     <col min="5" max="5" width="24.90625" customWidth="1"/>
+    <col min="6" max="6" width="69.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -462,12 +463,12 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -484,7 +485,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -499,12 +500,12 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -521,7 +522,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -552,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
         <v>30</v>
@@ -577,7 +578,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -594,7 +595,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -611,7 +612,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -619,12 +620,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.35">
@@ -632,47 +633,47 @@
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>